<commit_message>
maj tab liste entreprises
</commit_message>
<xml_diff>
--- a/Recheche stage/Liste entreprises.xlsx
+++ b/Recheche stage/Liste entreprises.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Nom Entreprise</t>
   </si>
@@ -31,15 +31,112 @@
   </si>
   <si>
     <t>Réponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORD SERVICE TELEMATIQUE SARL</t>
+  </si>
+  <si>
+    <t>LILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par sponteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIZZDEV FRANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY DEVELOPPEMENT</t>
+  </si>
+  <si>
+    <t>ALTEO</t>
+  </si>
+  <si>
+    <t>NORDSOFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VILLENEUVE D'ASCQ</t>
+  </si>
+  <si>
+    <t>UNIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTER WAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INEAT CONSEIL</t>
+  </si>
+  <si>
+    <t>EUROPRODUCTIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUSINESS APTITUDE</t>
+  </si>
+  <si>
+    <t>LEZENNES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATIVE INGENIERIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SII (SOCIETE POUR L'INFORMATIQUE INDUSTRIEL)</t>
+  </si>
+  <si>
+    <t>INOUIT</t>
+  </si>
+  <si>
+    <t>ELOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APSIDE NORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKKA I&amp;S</t>
+  </si>
+  <si>
+    <t>DEVOTEAM</t>
+  </si>
+  <si>
+    <t>NIJI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA MADELEINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAITEMENT ET GESTION INFORMATIQUE (TGI Maritime Software)</t>
+  </si>
+  <si>
+    <t>DUNKERQUE</t>
+  </si>
+  <si>
+    <t>NEXTOO</t>
+  </si>
+  <si>
+    <t>ROUBAIX</t>
+  </si>
+  <si>
+    <t>SFEIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA COOPERATIVE DES TILLEULS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
       <color theme="1"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
@@ -53,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -71,6 +168,19 @@
       <top style="thick">
         <color theme="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
       <bottom style="thick">
         <color theme="1"/>
       </bottom>
@@ -114,11 +224,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
@@ -157,35 +293,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,11 +883,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="16.7109375"/>
+  </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
@@ -711,506 +903,682 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9">
+        <v>44934</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="5"/>
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="5"/>
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="16"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="5"/>
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="10"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="5"/>
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="10"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="16"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="10"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="16"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="5"/>
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="16"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="5"/>
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="5"/>
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="16"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="5"/>
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="16"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="5"/>
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="16"/>
+    </row>
+    <row r="13" ht="32.25" customHeight="1">
+      <c r="A13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="16"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="5"/>
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="16"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="5"/>
+      <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="16"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="5"/>
+      <c r="A16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="16"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="5"/>
+      <c r="A17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="10"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="16"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="5"/>
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="10"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="16"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="5"/>
+      <c r="A19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="16"/>
+    </row>
+    <row r="20" ht="51.75" customHeight="1">
+      <c r="A20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="10"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="5"/>
+      <c r="A21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="5"/>
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="16"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="5"/>
+      <c r="A23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="17">
+        <v>44934</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" s="10"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="16"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="5"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="16"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="5"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="150">

</xml_diff>

<commit_message>
mise à jour liste entreprise
</commit_message>
<xml_diff>
--- a/Recheche stage/Liste entreprises.xlsx
+++ b/Recheche stage/Liste entreprises.xlsx
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -141,19 +141,19 @@
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="0" tint="0"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="34">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,40 +376,40 @@
     <xf fontId="0" fillId="0" borderId="12" numFmtId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="10" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="11" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="11" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="12" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="12" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -420,42 +420,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="10" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="11" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="12" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1232,32 +1196,34 @@
       <c r="R9" s="30"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="16">
-        <v>44934</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="15"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22">
+        <v>44934</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -1602,34 +1568,34 @@
       <c r="R22" s="15"/>
     </row>
     <row r="23">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="34" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37">
-        <v>44934</v>
-      </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" s="41"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="43" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22">
+        <v>44934</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="45"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="30"/>
     </row>
     <row r="24">
       <c r="A24" s="15"/>

</xml_diff>

<commit_message>
bon cv dans le dossier cv + maj tab liste entreprise
</commit_message>
<xml_diff>
--- a/Recheche stage/Liste entreprises.xlsx
+++ b/Recheche stage/Liste entreprises.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">Nom Entreprise</t>
   </si>
@@ -121,13 +121,22 @@
   </si>
   <si>
     <t xml:space="preserve">LA COOPERATIVE DES TILLEULS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEMN (CNRS)</t>
+  </si>
+  <si>
+    <t>billel.guerboukha@iemn.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -146,6 +155,12 @@
       <color theme="0" tint="0"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="10"/>
+      <sz val="11.000000"/>
+      <u/>
     </font>
   </fonts>
   <fills count="3">
@@ -320,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,6 +435,18 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,7 +955,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F13" zoomScale="100" workbookViewId="0">
       <selection activeCell="A9" activeCellId="0" sqref="A9:R9"/>
     </sheetView>
   </sheetViews>
@@ -1598,19 +1625,27 @@
       <c r="R23" s="30"/>
     </row>
     <row r="24">
-      <c r="A24" s="15"/>
+      <c r="A24" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="35" t="s">
+        <v>13</v>
+      </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
+      <c r="G24" s="36">
+        <v>44942</v>
+      </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="M24" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="N24" s="11"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
@@ -1790,6 +1825,9 @@
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="P25:R25"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="M24"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>